<commit_message>
fixed errors in csv resumes
</commit_message>
<xml_diff>
--- a/results/combined_output.xlsx
+++ b/results/combined_output.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO54"/>
+  <dimension ref="A1:AO62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11489,6 +11489,1646 @@
       <c r="AO54" t="inlineStr">
         <is>
           <t>0.627 (0.484)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Run1</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>0.170 (0.321)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0.219 (0.209)</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>0.149 (0.357)</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>0.198 (0.324)</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>0.314 (0.234)</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>0.139 (0.347)</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>0.068 (0.154)</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>0.225 (0.160)</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>0.011 (0.103)</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>0.269 (0.329)</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>0.561 (0.199)</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>0.050 (0.219)</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>0.405 (0.458)</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>0.795 (0.164)</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>0.287 (0.454)</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>0.204 (0.366)</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>0.295 (0.216)</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>0.184 (0.389)</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>0.418 (0.472)</t>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>0.128 (0.163)</t>
+        </is>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>0.516 (0.500)</t>
+        </is>
+      </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>0.143 (0.333)</t>
+        </is>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>0.289 (0.284)</t>
+        </is>
+      </c>
+      <c r="Z55" t="inlineStr">
+        <is>
+          <t>0.128 (0.334)</t>
+        </is>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>0.047 (0.129)</t>
+        </is>
+      </c>
+      <c r="AB55" t="inlineStr">
+        <is>
+          <t>0.289 (0.180)</t>
+        </is>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>0.000 (0.000)</t>
+        </is>
+      </c>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t>0.272 (0.395)</t>
+        </is>
+      </c>
+      <c r="AE55" t="inlineStr">
+        <is>
+          <t>0.281 (0.257)</t>
+        </is>
+      </c>
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t>0.267 (0.443)</t>
+        </is>
+      </c>
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t>0.218 (0.367)</t>
+        </is>
+      </c>
+      <c r="AH55" t="inlineStr">
+        <is>
+          <t>0.398 (0.296)</t>
+        </is>
+      </c>
+      <c r="AI55" t="inlineStr">
+        <is>
+          <t>0.162 (0.369)</t>
+        </is>
+      </c>
+      <c r="AJ55" t="inlineStr">
+        <is>
+          <t>0.086 (0.211)</t>
+        </is>
+      </c>
+      <c r="AK55" t="inlineStr">
+        <is>
+          <t>0.252 (0.177)</t>
+        </is>
+      </c>
+      <c r="AL55" t="inlineStr">
+        <is>
+          <t>0.040 (0.197)</t>
+        </is>
+      </c>
+      <c r="AM55" t="inlineStr">
+        <is>
+          <t>0.179 (0.247)</t>
+        </is>
+      </c>
+      <c r="AN55" t="inlineStr">
+        <is>
+          <t>0.368 (0.232)</t>
+        </is>
+      </c>
+      <c r="AO55" t="inlineStr">
+        <is>
+          <t>0.004 (0.066)</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Run2</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0.083 (0.197)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0.211 (0.201)</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0.029 (0.168)</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0.119 (0.243)</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>0.246 (0.224)</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>0.054 (0.227)</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>0.050 (0.117)</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0.170 (0.119)</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>0.006 (0.080)</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0.243 (0.307)</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>0.518 (0.203)</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>0.036 (0.186)</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>0.365 (0.441)</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>0.744 (0.171)</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>0.250 (0.434)</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>0.185 (0.345)</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>0.326 (0.201)</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>0.154 (0.362)</t>
+        </is>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>0.329 (0.440)</t>
+        </is>
+      </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t>0.171 (0.185)</t>
+        </is>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>0.382 (0.487)</t>
+        </is>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>0.037 (0.139)</t>
+        </is>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>0.353 (0.230)</t>
+        </is>
+      </c>
+      <c r="Z56" t="inlineStr">
+        <is>
+          <t>0.005 (0.070)</t>
+        </is>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>0.068 (0.183)</t>
+        </is>
+      </c>
+      <c r="AB56" t="inlineStr">
+        <is>
+          <t>0.291 (0.159)</t>
+        </is>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>0.024 (0.153)</t>
+        </is>
+      </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t>0.195 (0.337)</t>
+        </is>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t>0.279 (0.243)</t>
+        </is>
+      </c>
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t>0.158 (0.365)</t>
+        </is>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>0.136 (0.289)</t>
+        </is>
+      </c>
+      <c r="AH56" t="inlineStr">
+        <is>
+          <t>0.350 (0.287)</t>
+        </is>
+      </c>
+      <c r="AI56" t="inlineStr">
+        <is>
+          <t>0.071 (0.256)</t>
+        </is>
+      </c>
+      <c r="AJ56" t="inlineStr">
+        <is>
+          <t>0.081 (0.205)</t>
+        </is>
+      </c>
+      <c r="AK56" t="inlineStr">
+        <is>
+          <t>0.225 (0.159)</t>
+        </is>
+      </c>
+      <c r="AL56" t="inlineStr">
+        <is>
+          <t>0.041 (0.199)</t>
+        </is>
+      </c>
+      <c r="AM56" t="inlineStr">
+        <is>
+          <t>0.160 (0.231)</t>
+        </is>
+      </c>
+      <c r="AN56" t="inlineStr">
+        <is>
+          <t>0.326 (0.227)</t>
+        </is>
+      </c>
+      <c r="AO56" t="inlineStr">
+        <is>
+          <t>0.006 (0.076)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Run3</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0.205 (0.352)</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0.211 (0.188)</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0.203 (0.402)</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>0.157 (0.290)</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>0.252 (0.215)</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>0.108 (0.311)</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>0.175 (0.337)</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>0.180 (0.183)</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>0.173 (0.379)</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>0.344 (0.379)</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>0.594 (0.219)</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>0.157 (0.365)</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>0.427 (0.463)</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>0.801 (0.155)</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>0.314 (0.465)</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>0.480 (0.472)</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>0.331 (0.258)</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>0.512 (0.501)</t>
+        </is>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>0.539 (0.482)</t>
+        </is>
+      </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t>0.101 (0.154)</t>
+        </is>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>0.687 (0.465)</t>
+        </is>
+      </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>0.042 (0.158)</t>
+        </is>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>0.413 (0.270)</t>
+        </is>
+      </c>
+      <c r="Z57" t="inlineStr">
+        <is>
+          <t>0.005 (0.070)</t>
+        </is>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>0.154 (0.319)</t>
+        </is>
+      </c>
+      <c r="AB57" t="inlineStr">
+        <is>
+          <t>0.344 (0.224)</t>
+        </is>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>0.117 (0.322)</t>
+        </is>
+      </c>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t>0.343 (0.431)</t>
+        </is>
+      </c>
+      <c r="AE57" t="inlineStr">
+        <is>
+          <t>0.279 (0.268)</t>
+        </is>
+      </c>
+      <c r="AF57" t="inlineStr">
+        <is>
+          <t>0.371 (0.483)</t>
+        </is>
+      </c>
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t>0.168 (0.325)</t>
+        </is>
+      </c>
+      <c r="AH57" t="inlineStr">
+        <is>
+          <t>0.373 (0.298)</t>
+        </is>
+      </c>
+      <c r="AI57" t="inlineStr">
+        <is>
+          <t>0.105 (0.307)</t>
+        </is>
+      </c>
+      <c r="AJ57" t="inlineStr">
+        <is>
+          <t>0.224 (0.380)</t>
+        </is>
+      </c>
+      <c r="AK57" t="inlineStr">
+        <is>
+          <t>0.245 (0.220)</t>
+        </is>
+      </c>
+      <c r="AL57" t="inlineStr">
+        <is>
+          <t>0.218 (0.413)</t>
+        </is>
+      </c>
+      <c r="AM57" t="inlineStr">
+        <is>
+          <t>0.178 (0.267)</t>
+        </is>
+      </c>
+      <c r="AN57" t="inlineStr">
+        <is>
+          <t>0.344 (0.264)</t>
+        </is>
+      </c>
+      <c r="AO57" t="inlineStr">
+        <is>
+          <t>0.023 (0.151)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Run4</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0.258 (0.391)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0.216 (0.200)</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>0.276 (0.448)</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>0.204 (0.383)</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>0.059 (0.084)</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>0.278 (0.449)</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>0.156 (0.319)</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>0.156 (0.142)</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>0.156 (0.363)</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>0.257 (0.320)</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>0.532 (0.205)</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>0.050 (0.219)</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>0.299 (0.419)</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>0.775 (0.163)</t>
+        </is>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>0.154 (0.362)</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>0.322 (0.438)</t>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>0.292 (0.237)</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>0.328 (0.471)</t>
+        </is>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>0.583 (0.463)</t>
+        </is>
+      </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>0.195 (0.202)</t>
+        </is>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>0.713 (0.453)</t>
+        </is>
+      </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>0.089 (0.260)</t>
+        </is>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>0.342 (0.271)</t>
+        </is>
+      </c>
+      <c r="Z58" t="inlineStr">
+        <is>
+          <t>0.064 (0.245)</t>
+        </is>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>0.112 (0.272)</t>
+        </is>
+      </c>
+      <c r="AB58" t="inlineStr">
+        <is>
+          <t>0.276 (0.206)</t>
+        </is>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>0.080 (0.272)</t>
+        </is>
+      </c>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t>0.367 (0.433)</t>
+        </is>
+      </c>
+      <c r="AE58" t="inlineStr">
+        <is>
+          <t>0.291 (0.247)</t>
+        </is>
+      </c>
+      <c r="AF58" t="inlineStr">
+        <is>
+          <t>0.400 (0.490)</t>
+        </is>
+      </c>
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t>0.183 (0.362)</t>
+        </is>
+      </c>
+      <c r="AH58" t="inlineStr">
+        <is>
+          <t>0.226 (0.308)</t>
+        </is>
+      </c>
+      <c r="AI58" t="inlineStr">
+        <is>
+          <t>0.170 (0.376)</t>
+        </is>
+      </c>
+      <c r="AJ58" t="inlineStr">
+        <is>
+          <t>0.172 (0.338)</t>
+        </is>
+      </c>
+      <c r="AK58" t="inlineStr">
+        <is>
+          <t>0.207 (0.187)</t>
+        </is>
+      </c>
+      <c r="AL58" t="inlineStr">
+        <is>
+          <t>0.162 (0.369)</t>
+        </is>
+      </c>
+      <c r="AM58" t="inlineStr">
+        <is>
+          <t>0.157 (0.247)</t>
+        </is>
+      </c>
+      <c r="AN58" t="inlineStr">
+        <is>
+          <t>0.306 (0.253)</t>
+        </is>
+      </c>
+      <c r="AO58" t="inlineStr">
+        <is>
+          <t>0.019 (0.136)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>0</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Run5</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0.181 (0.349)</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0.130 (0.158)</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0.203 (0.402)</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0.065 (0.160)</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>0.146 (0.143)</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>0.024 (0.152)</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>0.076 (0.200)</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>0.154 (0.134)</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>0.047 (0.212)</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>0.328 (0.370)</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>0.603 (0.208)</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>0.121 (0.328)</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>0.558 (0.466)</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>0.786 (0.196)</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>0.489 (0.501)</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>0.585 (0.465)</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>0.327 (0.263)</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>0.642 (0.481)</t>
+        </is>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>0.030 (0.103)</t>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>0.102 (0.134)</t>
+        </is>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>0.006 (0.077)</t>
+        </is>
+      </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>0.023 (0.092)</t>
+        </is>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>0.226 (0.155)</t>
+        </is>
+      </c>
+      <c r="Z59" t="inlineStr">
+        <is>
+          <t>0.002 (0.050)</t>
+        </is>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>0.135 (0.299)</t>
+        </is>
+      </c>
+      <c r="AB59" t="inlineStr">
+        <is>
+          <t>0.325 (0.221)</t>
+        </is>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>0.099 (0.299)</t>
+        </is>
+      </c>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t>0.157 (0.313)</t>
+        </is>
+      </c>
+      <c r="AE59" t="inlineStr">
+        <is>
+          <t>0.244 (0.269)</t>
+        </is>
+      </c>
+      <c r="AF59" t="inlineStr">
+        <is>
+          <t>0.119 (0.324)</t>
+        </is>
+      </c>
+      <c r="AG59" t="inlineStr">
+        <is>
+          <t>0.142 (0.307)</t>
+        </is>
+      </c>
+      <c r="AH59" t="inlineStr">
+        <is>
+          <t>0.273 (0.289)</t>
+        </is>
+      </c>
+      <c r="AI59" t="inlineStr">
+        <is>
+          <t>0.101 (0.302)</t>
+        </is>
+      </c>
+      <c r="AJ59" t="inlineStr">
+        <is>
+          <t>0.190 (0.353)</t>
+        </is>
+      </c>
+      <c r="AK59" t="inlineStr">
+        <is>
+          <t>0.224 (0.200)</t>
+        </is>
+      </c>
+      <c r="AL59" t="inlineStr">
+        <is>
+          <t>0.180 (0.384)</t>
+        </is>
+      </c>
+      <c r="AM59" t="inlineStr">
+        <is>
+          <t>0.164 (0.256)</t>
+        </is>
+      </c>
+      <c r="AN59" t="inlineStr">
+        <is>
+          <t>0.317 (0.261)</t>
+        </is>
+      </c>
+      <c r="AO59" t="inlineStr">
+        <is>
+          <t>0.022 (0.146)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>0</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Run6</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0.123 (0.265)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0.202 (0.189)</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0.089 (0.285)</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>0.192 (0.362)</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>0.096 (0.124)</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>0.241 (0.428)</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>0.055 (0.136)</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>0.187 (0.165)</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>0.006 (0.080)</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>0.264 (0.329)</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>0.529 (0.219)</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>0.064 (0.246)</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>0.581 (0.462)</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>0.796 (0.174)</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>0.516 (0.501)</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>0.146 (0.307)</t>
+        </is>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>0.312 (0.211)</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>0.109 (0.313)</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>0.382 (0.469)</t>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>0.099 (0.153)</t>
+        </is>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>0.478 (0.500)</t>
+        </is>
+      </c>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>0.212 (0.397)</t>
+        </is>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>0.220 (0.261)</t>
+        </is>
+      </c>
+      <c r="Z60" t="inlineStr">
+        <is>
+          <t>0.211 (0.409)</t>
+        </is>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>0.044 (0.122)</t>
+        </is>
+      </c>
+      <c r="AB60" t="inlineStr">
+        <is>
+          <t>0.254 (0.159)</t>
+        </is>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>0.003 (0.052)</t>
+        </is>
+      </c>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t>0.236 (0.375)</t>
+        </is>
+      </c>
+      <c r="AE60" t="inlineStr">
+        <is>
+          <t>0.257 (0.250)</t>
+        </is>
+      </c>
+      <c r="AF60" t="inlineStr">
+        <is>
+          <t>0.226 (0.419)</t>
+        </is>
+      </c>
+      <c r="AG60" t="inlineStr">
+        <is>
+          <t>0.270 (0.420)</t>
+        </is>
+      </c>
+      <c r="AH60" t="inlineStr">
+        <is>
+          <t>0.239 (0.309)</t>
+        </is>
+      </c>
+      <c r="AI60" t="inlineStr">
+        <is>
+          <t>0.280 (0.449)</t>
+        </is>
+      </c>
+      <c r="AJ60" t="inlineStr">
+        <is>
+          <t>0.068 (0.180)</t>
+        </is>
+      </c>
+      <c r="AK60" t="inlineStr">
+        <is>
+          <t>0.223 (0.177)</t>
+        </is>
+      </c>
+      <c r="AL60" t="inlineStr">
+        <is>
+          <t>0.025 (0.156)</t>
+        </is>
+      </c>
+      <c r="AM60" t="inlineStr">
+        <is>
+          <t>0.149 (0.234)</t>
+        </is>
+      </c>
+      <c r="AN60" t="inlineStr">
+        <is>
+          <t>0.305 (0.250)</t>
+        </is>
+      </c>
+      <c r="AO60" t="inlineStr">
+        <is>
+          <t>0.004 (0.066)</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Run7</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.176 (0.325)</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0.233 (0.214)</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0.151 (0.359)</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>0.177 (0.336)</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>0.144 (0.163)</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>0.193 (0.395)</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>0.138 (0.293)</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>0.194 (0.179)</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>0.118 (0.322)</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>0.318 (0.364)</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>0.571 (0.216)</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>0.129 (0.336)</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>0.446 (0.462)</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>0.777 (0.164)</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>0.346 (0.477)</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>0.319 (0.432)</t>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>0.324 (0.215)</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>0.318 (0.467)</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>0.429 (0.483)</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>0.071 (0.128)</t>
+        </is>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>0.549 (0.498)</t>
+        </is>
+      </c>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>0.117 (0.300)</t>
+        </is>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>0.324 (0.270)</t>
+        </is>
+      </c>
+      <c r="Z61" t="inlineStr">
+        <is>
+          <t>0.096 (0.295)</t>
+        </is>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t>0.129 (0.292)</t>
+        </is>
+      </c>
+      <c r="AB61" t="inlineStr">
+        <is>
+          <t>0.296 (0.209)</t>
+        </is>
+      </c>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t>0.096 (0.295)</t>
+        </is>
+      </c>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t>0.287 (0.407)</t>
+        </is>
+      </c>
+      <c r="AE61" t="inlineStr">
+        <is>
+          <t>0.275 (0.269)</t>
+        </is>
+      </c>
+      <c r="AF61" t="inlineStr">
+        <is>
+          <t>0.292 (0.455)</t>
+        </is>
+      </c>
+      <c r="AG61" t="inlineStr">
+        <is>
+          <t>0.206 (0.370)</t>
+        </is>
+      </c>
+      <c r="AH61" t="inlineStr">
+        <is>
+          <t>0.282 (0.301)</t>
+        </is>
+      </c>
+      <c r="AI61" t="inlineStr">
+        <is>
+          <t>0.183 (0.386)</t>
+        </is>
+      </c>
+      <c r="AJ61" t="inlineStr">
+        <is>
+          <t>0.168 (0.330)</t>
+        </is>
+      </c>
+      <c r="AK61" t="inlineStr">
+        <is>
+          <t>0.239 (0.200)</t>
+        </is>
+      </c>
+      <c r="AL61" t="inlineStr">
+        <is>
+          <t>0.148 (0.356)</t>
+        </is>
+      </c>
+      <c r="AM61" t="inlineStr">
+        <is>
+          <t>0.184 (0.269)</t>
+        </is>
+      </c>
+      <c r="AN61" t="inlineStr">
+        <is>
+          <t>0.351 (0.258)</t>
+        </is>
+      </c>
+      <c r="AO61" t="inlineStr">
+        <is>
+          <t>0.029 (0.168)</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>0</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Run8</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0.214 (0.357)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0.246 (0.221)</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0.200 (0.401)</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>0.110 (0.258)</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>0.126 (0.131)</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>0.101 (0.302)</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>0.046 (0.091)</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>0.169 (0.098)</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>0.000 (0.000)</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>0.251 (0.314)</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>0.547 (0.199)</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>0.029 (0.167)</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>0.445 (0.461)</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>0.755 (0.179)</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>0.351 (0.479)</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>0.081 (0.209)</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>0.291 (0.187)</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>0.035 (0.184)</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>0.128 (0.283)</t>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>0.199 (0.179)</t>
+        </is>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>0.104 (0.306)</t>
+        </is>
+      </c>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>0.058 (0.193)</t>
+        </is>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>0.415 (0.224)</t>
+        </is>
+      </c>
+      <c r="Z62" t="inlineStr">
+        <is>
+          <t>0.022 (0.147)</t>
+        </is>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>0.032 (0.090)</t>
+        </is>
+      </c>
+      <c r="AB62" t="inlineStr">
+        <is>
+          <t>0.197 (0.132)</t>
+        </is>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>0.000 (0.000)</t>
+        </is>
+      </c>
+      <c r="AD62" t="inlineStr">
+        <is>
+          <t>0.192 (0.329)</t>
+        </is>
+      </c>
+      <c r="AE62" t="inlineStr">
+        <is>
+          <t>0.310 (0.248)</t>
+        </is>
+      </c>
+      <c r="AF62" t="inlineStr">
+        <is>
+          <t>0.140 (0.347)</t>
+        </is>
+      </c>
+      <c r="AG62" t="inlineStr">
+        <is>
+          <t>0.154 (0.321)</t>
+        </is>
+      </c>
+      <c r="AH62" t="inlineStr">
+        <is>
+          <t>0.278 (0.289)</t>
+        </is>
+      </c>
+      <c r="AI62" t="inlineStr">
+        <is>
+          <t>0.116 (0.320)</t>
+        </is>
+      </c>
+      <c r="AJ62" t="inlineStr">
+        <is>
+          <t>0.047 (0.122)</t>
+        </is>
+      </c>
+      <c r="AK62" t="inlineStr">
+        <is>
+          <t>0.195 (0.130)</t>
+        </is>
+      </c>
+      <c r="AL62" t="inlineStr">
+        <is>
+          <t>0.007 (0.082)</t>
+        </is>
+      </c>
+      <c r="AM62" t="inlineStr">
+        <is>
+          <t>0.149 (0.224)</t>
+        </is>
+      </c>
+      <c r="AN62" t="inlineStr">
+        <is>
+          <t>0.309 (0.234)</t>
+        </is>
+      </c>
+      <c r="AO62" t="inlineStr">
+        <is>
+          <t>0.000 (0.000)</t>
         </is>
       </c>
     </row>
@@ -11532,7 +13172,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0.60 (0.04)</t>
+          <t>0.51 (0.20)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -11547,7 +13187,7 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>0.72 (0.07)</t>
+          <t>0.62 (0.15)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -11562,7 +13202,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>0.55 (0.03)</t>
+          <t>0.62 (0.15)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
@@ -11577,7 +13217,7 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>0.64 (0.04)</t>
+          <t>0.69 (0.22)</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
@@ -11592,7 +13232,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>0.82 (0.02)</t>
+          <t>0.73 (0.13)</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -11607,7 +13247,7 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>0.62 (0.08)</t>
+          <t>0.71 (0.26)</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
@@ -11622,7 +13262,7 @@
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>0.59 (0.08)</t>
+          <t>0.73 (0.16)</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
@@ -11637,7 +13277,7 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>0.61 (0.06)</t>
+          <t>0.80 (0.07)</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
@@ -11652,7 +13292,7 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>0.53 (0.04)</t>
+          <t>0.72 (0.20)</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
@@ -11662,12 +13302,12 @@
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>0.62 (0.11)</t>
+          <t>0.60 (0.02)</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>0.62 (0.11)</t>
+          <t>0.62 (0.16)</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
@@ -11677,12 +13317,12 @@
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>0.71 (0.09)</t>
+          <t>0.72 (0.04)</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>0.71 (0.09)</t>
+          <t>0.71 (0.11)</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
@@ -11692,12 +13332,12 @@
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>0.65 (0.14)</t>
+          <t>0.56 (0.01)</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>0.65 (0.14)</t>
+          <t>0.67 (0.18)</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
@@ -11737,157 +13377,157 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>0.47 (0.12)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.79 (0.02)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.78 (0.00)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.80 (0.03)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.65 (0.04)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.53 (0.06)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.69 (0.04)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.77 (0.11)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0.66 (0.04)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.85 (0.17)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.83 (0.02)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0.82 (0.01)</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>0.84 (0.03)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>0.82 (0.03)</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>0.72 (0.03)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0.84 (0.04)</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0.79 (0.07)</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>0.58 (0.02)</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>0.86 (0.09)</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>0.89 (0.02)</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>0.66 (0.02)</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>0.91 (0.02)</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>0.81 (0.04)</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>0.55 (0.04)</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>0.86 (0.05)</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>0.65 (0.08)</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
           <t>0.61 (0.02)</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0.79 (0.02)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.78 (0.00)</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.78 (0.00)</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.65 (0.04)</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.53 (0.06)</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0.53 (0.06)</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>0.77 (0.11)</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0.66 (0.04)</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>0.66 (0.04)</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>0.67 (0.12)</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
         <is>
           <t>0.83 (0.02)</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>0.82 (0.01)</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0.82 (0.01)</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0.82 (0.03)</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>0.72 (0.03)</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>0.72 (0.03)</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>0.79 (0.07)</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>0.58 (0.02)</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0.58 (0.02)</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>0.89 (0.02)</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>0.66 (0.02)</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>0.66 (0.02)</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>0.81 (0.04)</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>0.55 (0.04)</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>0.55 (0.04)</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>0.65 (0.08)</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>0.65 (0.08)</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>0.65 (0.08)</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>0.83 (0.02)</t>
-        </is>
-      </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>0.83 (0.02)</t>
+          <t>0.77 (0.00)</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>0.83 (0.02)</t>
+          <t>0.85 (0.02)</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
@@ -11897,12 +13537,12 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>0.73 (0.03)</t>
+          <t>0.56 (0.03)</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>0.73 (0.03)</t>
+          <t>0.78 (0.03)</t>
         </is>
       </c>
       <c r="AM2" t="inlineStr">
@@ -11942,7 +13582,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.51 (0.04)</t>
+          <t>0.75 (0.09)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -11957,7 +13597,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.73 (0.01)</t>
+          <t>0.76 (0.11)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -11972,142 +13612,142 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>0.62 (0.08)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.66 (0.02)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.60 (0.01)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.69 (0.02)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0.83 (0.06)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0.86 (0.01)</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0.82 (0.08)</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0.75 (0.02)</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
           <t>0.60 (0.02)</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0.66 (0.02)</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0.82 (0.03)</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0.80 (0.07)</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>0.67 (0.03)</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>0.83 (0.08)</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>0.85 (0.02)</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>0.67 (0.04)</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>0.88 (0.02)</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>0.76 (0.02)</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>0.59 (0.03)</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>0.83 (0.04)</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>0.72 (0.05)</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>0.57 (0.03)</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>0.77 (0.07)</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>0.80 (0.05)</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>0.74 (0.01)</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>0.82 (0.06)</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>0.69 (0.04)</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
         <is>
           <t>0.60 (0.01)</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>0.60 (0.01)</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>0.83 (0.06)</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>0.86 (0.01)</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0.86 (0.01)</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0.75 (0.02)</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>0.60 (0.02)</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>0.60 (0.02)</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>0.80 (0.07)</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>0.67 (0.03)</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>0.67 (0.03)</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>0.85 (0.02)</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>0.67 (0.04)</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>0.67 (0.04)</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>0.76 (0.02)</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>0.59 (0.03)</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>0.59 (0.03)</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>0.72 (0.05)</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>0.72 (0.05)</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>0.72 (0.05)</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>0.80 (0.05)</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>0.80 (0.05)</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>0.80 (0.05)</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>0.69 (0.04)</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>0.69 (0.04)</t>
-        </is>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>0.69 (0.04)</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
@@ -12147,7 +13787,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.60 (0.04)</t>
+          <t>0.62 (0.19)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -12162,7 +13802,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.72 (0.08)</t>
+          <t>0.83 (0.03)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -12177,7 +13817,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.57 (0.01)</t>
+          <t>0.71 (0.11)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -12192,7 +13832,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.62 (0.05)</t>
+          <t>0.66 (0.09)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -12207,112 +13847,112 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
+          <t>0.78 (0.03)</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>0.74 (0.05)</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>0.66 (0.05)</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>0.76 (0.08)</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>0.71 (0.10)</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>0.59 (0.04)</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>0.75 (0.13)</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>0.82 (0.04)</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>0.64 (0.05)</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
           <t>0.84 (0.04)</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>0.74 (0.11)</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>0.58 (0.07)</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>0.77 (0.16)</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>0.65 (0.06)</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>0.60 (0.02)</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>0.67 (0.08)</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>0.81 (0.02)</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>0.75 (0.02)</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>0.83 (0.01)</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>0.71 (0.04)</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>0.60 (0.03)</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
         <is>
           <t>0.74 (0.05)</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>0.66 (0.05)</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>0.66 (0.05)</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>0.71 (0.10)</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>0.59 (0.04)</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>0.59 (0.04)</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>0.82 (0.04)</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>0.64 (0.05)</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>0.64 (0.05)</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>0.74 (0.11)</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>0.58 (0.07)</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>0.58 (0.07)</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>0.65 (0.06)</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>0.65 (0.06)</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>0.65 (0.06)</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>0.81 (0.02)</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>0.81 (0.02)</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>0.81 (0.02)</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>0.71 (0.04)</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>0.71 (0.04)</t>
-        </is>
-      </c>
-      <c r="AL4" t="inlineStr">
-        <is>
-          <t>0.71 (0.04)</t>
         </is>
       </c>
       <c r="AM4" t="inlineStr">
@@ -12352,7 +13992,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.62 (0.06)</t>
+          <t>0.57 (0.20)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -12367,7 +14007,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.73 (0.07)</t>
+          <t>0.78 (0.07)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -12382,7 +14022,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.58 (0.02)</t>
+          <t>0.62 (0.22)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -12397,7 +14037,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.63 (0.07)</t>
+          <t>0.67 (0.22)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -12412,7 +14052,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>0.84 (0.03)</t>
+          <t>0.82 (0.09)</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -12427,7 +14067,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>0.65 (0.06)</t>
+          <t>0.76 (0.13)</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -12442,7 +14082,7 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>0.57 (0.05)</t>
+          <t>0.75 (0.19)</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
@@ -12457,7 +14097,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>0.65 (0.10)</t>
+          <t>0.82 (0.14)</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
@@ -12472,7 +14112,7 @@
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>0.56 (0.08)</t>
+          <t>0.74 (0.16)</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
@@ -12482,12 +14122,12 @@
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>0.63 (0.11)</t>
+          <t>0.60 (0.02)</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>0.63 (0.11)</t>
+          <t>0.65 (0.15)</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
@@ -12497,12 +14137,12 @@
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>0.79 (0.07)</t>
+          <t>0.74 (0.03)</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>0.79 (0.07)</t>
+          <t>0.80 (0.08)</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
@@ -12512,12 +14152,12 @@
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>0.67 (0.11)</t>
+          <t>0.59 (0.03)</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>0.67 (0.11)</t>
+          <t>0.68 (0.14)</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
@@ -12557,7 +14197,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.60 (0.06)</t>
+          <t>0.55 (0.20)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -12572,7 +14212,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.75 (0.07)</t>
+          <t>0.79 (0.05)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -12587,7 +14227,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.55 (0.05)</t>
+          <t>0.72 (0.19)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -12602,7 +14242,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.63 (0.06)</t>
+          <t>0.64 (0.22)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -12617,7 +14257,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>0.84 (0.02)</t>
+          <t>0.84 (0.06)</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -12632,7 +14272,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>0.61 (0.15)</t>
+          <t>0.87 (0.03)</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -12647,7 +14287,7 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>0.57 (0.05)</t>
+          <t>0.75 (0.16)</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
@@ -12662,7 +14302,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>0.62 (0.04)</t>
+          <t>0.86 (0.09)</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
@@ -12677,7 +14317,7 @@
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>0.51 (0.08)</t>
+          <t>0.83 (0.09)</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
@@ -12687,12 +14327,12 @@
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>0.62 (0.10)</t>
+          <t>0.60 (0.03)</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>0.62 (0.10)</t>
+          <t>0.64 (0.14)</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -12702,12 +14342,12 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>0.81 (0.05)</t>
+          <t>0.74 (0.04)</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>0.81 (0.05)</t>
+          <t>0.83 (0.06)</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
@@ -12717,12 +14357,12 @@
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>0.73 (0.08)</t>
+          <t>0.56 (0.02)</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>0.73 (0.08)</t>
+          <t>0.78 (0.09)</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr">
@@ -12762,7 +14402,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.32 (0.05)</t>
+          <t>0.09 (0.03)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -12777,7 +14417,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.36 (0.19)</t>
+          <t>0.12 (0.06)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -12792,7 +14432,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.27 (0.12)</t>
+          <t>0.05 (0.08)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -12807,7 +14447,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.56 (0.03)</t>
+          <t>0.06 (0.04)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -12822,7 +14462,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>0.79 (0.07)</t>
+          <t>0.31 (0.18)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -12837,7 +14477,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>0.60 (0.02)</t>
+          <t>0.25 (0.24)</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -12852,7 +14492,7 @@
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>0.24 (0.17)</t>
+          <t>0.37 (0.06)</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
@@ -12867,7 +14507,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>0.44 (0.07)</t>
+          <t>0.51 (0.12)</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
@@ -12882,7 +14522,7 @@
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>0.37 (0.10)</t>
+          <t>0.07 (0.07)</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
@@ -12892,12 +14532,12 @@
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>0.24 (0.02)</t>
+          <t>0.34 (0.07)</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>0.24 (0.02)</t>
+          <t>0.20 (0.03)</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
@@ -12907,12 +14547,12 @@
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>0.34 (0.08)</t>
+          <t>0.49 (0.11)</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>0.34 (0.08)</t>
+          <t>0.31 (0.08)</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
@@ -12922,12 +14562,12 @@
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>0.15 (0.10)</t>
+          <t>0.38 (0.09)</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>0.15 (0.10)</t>
+          <t>0.09 (0.10)</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
@@ -12967,7 +14607,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.30 (0.12)</t>
+          <t>0.37 (0.21)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -12982,7 +14622,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.39 (0.12)</t>
+          <t>0.20 (0.05)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -12997,7 +14637,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.40 (0.14)</t>
+          <t>0.29 (0.28)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -13012,7 +14652,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.58 (0.02)</t>
+          <t>0.16 (0.10)</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -13027,7 +14667,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>0.82 (0.06)</t>
+          <t>0.38 (0.20)</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -13042,7 +14682,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>0.61 (0.03)</t>
+          <t>0.43 (0.18)</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -13057,7 +14697,7 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>0.30 (0.14)</t>
+          <t>0.50 (0.26)</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
@@ -13072,7 +14712,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>0.47 (0.13)</t>
+          <t>0.66 (0.17)</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
@@ -13087,7 +14727,7 @@
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>0.52 (0.14)</t>
+          <t>0.33 (0.28)</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
@@ -13097,12 +14737,12 @@
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>0.38 (0.13)</t>
+          <t>0.36 (0.06)</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>0.38 (0.13)</t>
+          <t>0.39 (0.17)</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
@@ -13112,12 +14752,12 @@
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>0.44 (0.10)</t>
+          <t>0.53 (0.12)</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
         <is>
-          <t>0.44 (0.10)</t>
+          <t>0.42 (0.10)</t>
         </is>
       </c>
       <c r="AJ8" t="inlineStr">
@@ -13127,12 +14767,12 @@
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>0.36 (0.22)</t>
+          <t>0.48 (0.13)</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>0.36 (0.22)</t>
+          <t>0.33 (0.25)</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr">
@@ -13172,7 +14812,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.53 (0.06)</t>
+          <t>0.26 (0.22)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -13187,7 +14827,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.45 (0.15)</t>
+          <t>0.46 (0.14)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -13202,7 +14842,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.44 (0.12)</t>
+          <t>0.44 (0.19)</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -13217,7 +14857,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.56 (0.03)</t>
+          <t>0.43 (0.06)</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -13232,7 +14872,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>0.78 (0.04)</t>
+          <t>0.55 (0.15)</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -13247,67 +14887,67 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
+          <t>0.43 (0.20)</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0.45 (0.20)</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>0.52 (0.11)</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>0.42 (0.24)</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>0.65 (0.09)</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>0.57 (0.06)</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>0.66 (0.11)</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>0.52 (0.18)</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>0.49 (0.09)</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>0.53 (0.24)</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>0.41 (0.13)</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
           <t>0.53 (0.03)</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>0.45 (0.20)</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t>0.52 (0.11)</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>0.52 (0.11)</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>0.65 (0.09)</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>0.57 (0.06)</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>0.57 (0.06)</t>
-        </is>
-      </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>0.52 (0.18)</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>0.49 (0.09)</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>0.49 (0.09)</t>
-        </is>
-      </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t>0.41 (0.13)</t>
-        </is>
-      </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>0.41 (0.13)</t>
-        </is>
-      </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>0.41 (0.13)</t>
+          <t>0.35 (0.19)</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
@@ -13317,12 +14957,12 @@
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>0.56 (0.09)</t>
+          <t>0.60 (0.03)</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr">
         <is>
-          <t>0.56 (0.09)</t>
+          <t>0.56 (0.12)</t>
         </is>
       </c>
       <c r="AJ9" t="inlineStr">
@@ -13332,12 +14972,12 @@
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>0.47 (0.16)</t>
+          <t>0.48 (0.08)</t>
         </is>
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>0.47 (0.16)</t>
+          <t>0.47 (0.19)</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr">
@@ -13377,7 +15017,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.59 (0.09)</t>
+          <t>0.61 (0.25)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -13392,7 +15032,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.68 (0.09)</t>
+          <t>0.71 (0.15)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -13407,7 +15047,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.52 (0.11)</t>
+          <t>0.59 (0.29)</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -13422,7 +15062,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.61 (0.07)</t>
+          <t>0.68 (0.20)</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -13437,7 +15077,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>0.82 (0.05)</t>
+          <t>0.75 (0.17)</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -13452,7 +15092,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>0.62 (0.05)</t>
+          <t>0.64 (0.17)</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -13467,7 +15107,7 @@
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>0.55 (0.07)</t>
+          <t>0.66 (0.21)</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
@@ -13482,7 +15122,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>0.67 (0.04)</t>
+          <t>0.81 (0.08)</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
@@ -13497,7 +15137,7 @@
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>0.51 (0.13)</t>
+          <t>0.65 (0.18)</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
@@ -13507,12 +15147,12 @@
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>0.61 (0.15)</t>
+          <t>0.58 (0.06)</t>
         </is>
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>0.61 (0.15)</t>
+          <t>0.64 (0.20)</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr">
@@ -13522,12 +15162,12 @@
       </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>0.75 (0.10)</t>
+          <t>0.72 (0.05)</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr">
         <is>
-          <t>0.75 (0.10)</t>
+          <t>0.76 (0.11)</t>
         </is>
       </c>
       <c r="AJ10" t="inlineStr">
@@ -13537,12 +15177,12 @@
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>0.61 (0.18)</t>
+          <t>0.54 (0.11)</t>
         </is>
       </c>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>0.61 (0.18)</t>
+          <t>0.62 (0.22)</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr">

</xml_diff>

<commit_message>
added more results from iteration 24 #94
</commit_message>
<xml_diff>
--- a/results/combined_output.xlsx
+++ b/results/combined_output.xlsx
@@ -429,67 +429,67 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Run079</t>
+          <t>Run083</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0.661 (0.421)</t>
+          <t>0.432 (0.428)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>0.802 (0.143)</t>
+          <t>0.498 (0.128)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0.590 (0.492)</t>
+          <t>0.408 (0.492)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>0.856 (0.313)</t>
+          <t>0.602 (0.463)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>0.856 (0.123)</t>
+          <t>0.789 (0.164)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>0.856 (0.352)</t>
+          <t>0.560 (0.498)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>0.913 (0.252)</t>
+          <t>0.752 (0.395)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>0.637 (0.246)</t>
+          <t>0.683 (0.164)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>0.941 (0.236)</t>
+          <t>0.765 (0.424)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>0.782 (0.372)</t>
+          <t>0.571 (0.447)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>0.790 (0.169)</t>
+          <t>0.590 (0.184)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>0.779 (0.415)</t>
+          <t>0.566 (0.496)</t>
         </is>
       </c>
     </row>
@@ -499,67 +499,67 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Run080</t>
+          <t>Run084</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.675 (0.408)</t>
+          <t>0.308 (0.417)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.626 (0.188)</t>
+          <t>0.617 (0.203)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.693 (0.462)</t>
+          <t>0.229 (0.421)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.761 (0.405)</t>
+          <t>0.532 (0.446)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.909 (0.097)</t>
+          <t>0.735 (0.186)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.714 (0.453)</t>
+          <t>0.437 (0.498)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.896 (0.260)</t>
+          <t>0.625 (0.427)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.706 (0.155)</t>
+          <t>0.715 (0.171)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.927 (0.260)</t>
+          <t>0.585 (0.493)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0.771 (0.373)</t>
+          <t>0.463 (0.450)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.701 (0.198)</t>
+          <t>0.684 (0.193)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.790 (0.407)</t>
+          <t>0.386 (0.487)</t>
         </is>
       </c>
     </row>
@@ -569,67 +569,67 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Run081</t>
+          <t>Run085</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.897 (0.291)</t>
+          <t>0.638 (0.448)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.629 (0.318)</t>
+          <t>0.655 (0.107)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.913 (0.283)</t>
+          <t>0.635 (0.482)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.923 (0.205)</t>
+          <t>0.577 (0.421)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.866 (0.147)</t>
+          <t>0.767 (0.120)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.948 (0.223)</t>
+          <t>0.443 (0.499)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.875 (0.287)</t>
+          <t>0.686 (0.411)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.857 (0.095)</t>
+          <t>0.767 (0.146)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.880 (0.325)</t>
+          <t>0.653 (0.477)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.891 (0.280)</t>
+          <t>0.651 (0.430)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.829 (0.174)</t>
+          <t>0.738 (0.140)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.904 (0.295)</t>
+          <t>0.622 (0.485)</t>
         </is>
       </c>
     </row>
@@ -639,67 +639,67 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Run082</t>
+          <t>Run086</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.790 (0.384)</t>
+          <t>0.488 (0.466)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.876 (0.069)</t>
+          <t>0.641 (0.236)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.770 (0.421)</t>
+          <t>0.452 (0.498)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.843 (0.314)</t>
+          <t>0.504 (0.466)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.826 (0.189)</t>
+          <t>0.784 (0.119)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.850 (0.358)</t>
+          <t>0.427 (0.496)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.934 (0.221)</t>
+          <t>0.684 (0.436)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.731 (0.127)</t>
+          <t>0.514 (0.178)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.949 (0.219)</t>
+          <t>0.707 (0.455)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0.852 (0.327)</t>
+          <t>0.563 (0.464)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.837 (0.139)</t>
+          <t>0.640 (0.221)</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.855 (0.353)</t>
+          <t>0.547 (0.498)</t>
         </is>
       </c>
     </row>
@@ -728,67 +728,67 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Iteration23</t>
+          <t>Iteration24</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0.76 (0.10)</t>
+          <t>0.47 (0.12)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>0.73 (0.11)</t>
+          <t>0.60 (0.06)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0.74 (0.12)</t>
+          <t>0.43 (0.14)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>0.85 (0.06)</t>
+          <t>0.55 (0.04)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>0.86 (0.03)</t>
+          <t>0.77 (0.02)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>0.84 (0.08)</t>
+          <t>0.47 (0.05)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>0.90 (0.02)</t>
+          <t>0.69 (0.05)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>0.73 (0.08)</t>
+          <t>0.67 (0.09)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>0.92 (0.03)</t>
+          <t>0.68 (0.07)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>0.82 (0.05)</t>
+          <t>0.56 (0.07)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>0.79 (0.05)</t>
+          <t>0.66 (0.05)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>0.83 (0.05)</t>
+          <t>0.53 (0.09)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
results from the iterations 22 to 24 due to problem in testing
</commit_message>
<xml_diff>
--- a/results/combined_output.xlsx
+++ b/results/combined_output.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,67 +429,67 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Run083</t>
+          <t>Run075</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0.432 (0.428)</t>
+          <t>0.654 (0.412)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>0.498 (0.128)</t>
+          <t>0.663 (0.246)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0.408 (0.492)</t>
+          <t>0.649 (0.478)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>0.602 (0.463)</t>
+          <t>0.541 (0.386)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>0.789 (0.164)</t>
+          <t>0.606 (0.218)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>0.560 (0.498)</t>
+          <t>0.470 (0.501)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>0.752 (0.395)</t>
+          <t>0.648 (0.409)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>0.683 (0.164)</t>
+          <t>0.619 (0.196)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>0.765 (0.424)</t>
+          <t>0.661 (0.474)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>0.571 (0.447)</t>
+          <t>0.632 (0.408)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>0.590 (0.184)</t>
+          <t>0.635 (0.225)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>0.566 (0.496)</t>
+          <t>0.630 (0.483)</t>
         </is>
       </c>
     </row>
@@ -499,67 +499,67 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Run084</t>
+          <t>Run076</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.308 (0.417)</t>
+          <t>0.507 (0.428)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.617 (0.203)</t>
+          <t>0.641 (0.157)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.229 (0.421)</t>
+          <t>0.442 (0.497)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.532 (0.446)</t>
+          <t>0.741 (0.338)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.735 (0.186)</t>
+          <t>0.670 (0.179)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.437 (0.498)</t>
+          <t>0.791 (0.408)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.625 (0.427)</t>
+          <t>0.775 (0.379)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.715 (0.171)</t>
+          <t>0.675 (0.221)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.585 (0.493)</t>
+          <t>0.797 (0.403)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0.463 (0.450)</t>
+          <t>0.649 (0.418)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.684 (0.193)</t>
+          <t>0.656 (0.180)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.386 (0.487)</t>
+          <t>0.646 (0.478)</t>
         </is>
       </c>
     </row>
@@ -569,67 +569,67 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Run085</t>
+          <t>Run077</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.638 (0.448)</t>
+          <t>0.583 (0.455)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.655 (0.107)</t>
+          <t>0.516 (0.279)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.635 (0.482)</t>
+          <t>0.601 (0.490)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.577 (0.421)</t>
+          <t>0.689 (0.344)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.767 (0.120)</t>
+          <t>0.660 (0.184)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.443 (0.499)</t>
+          <t>0.719 (0.451)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.686 (0.411)</t>
+          <t>0.310 (0.419)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.767 (0.146)</t>
+          <t>0.451 (0.251)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.653 (0.477)</t>
+          <t>0.272 (0.446)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.651 (0.430)</t>
+          <t>0.502 (0.450)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.738 (0.140)</t>
+          <t>0.546 (0.256)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.622 (0.485)</t>
+          <t>0.486 (0.500)</t>
         </is>
       </c>
     </row>
@@ -639,67 +639,627 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Run078</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.618 (0.419)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.566 (0.248)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.643 (0.480)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.644 (0.433)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.686 (0.127)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.632 (0.483)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.588 (0.417)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.600 (0.198)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.582 (0.494)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0.611 (0.421)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0.594 (0.220)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.619 (0.486)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Run079</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.634 (0.451)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.798 (0.127)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.593 (0.492)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.791 (0.366)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.811 (0.183)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.783 (0.413)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.719 (0.422)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.696 (0.273)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.724 (0.448)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.693 (0.430)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0.768 (0.203)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.673 (0.469)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Run080</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.590 (0.405)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.642 (0.190)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.556 (0.497)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.864 (0.307)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.855 (0.157)</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0.867 (0.340)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.856 (0.300)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.706 (0.163)</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.890 (0.314)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.736 (0.378)</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0.686 (0.194)</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.756 (0.430)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Run081</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.821 (0.357)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.603 (0.266)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.850 (0.358)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.694 (0.409)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.779 (0.173)</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.654 (0.477)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.859 (0.334)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.555 (0.336)</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.882 (0.323)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.819 (0.359)</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>0.654 (0.272)</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0.843 (0.364)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Run082</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.487 (0.474)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.602 (0.180)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.471 (0.500)</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.815 (0.343)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.798 (0.213)</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.822 (0.384)</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.876 (0.285)</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.689 (0.190)</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.910 (0.287)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.687 (0.433)</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0.693 (0.209)</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0.686 (0.464)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Run083</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.398 (0.419)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.475 (0.139)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.369 (0.483)</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.683 (0.394)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.644 (0.189)</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0.701 (0.459)</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.607 (0.419)</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.566 (0.194)</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.625 (0.485)</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.525 (0.431)</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0.541 (0.183)</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>0.518 (0.500)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Run084</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.283 (0.418)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.504 (0.246)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.244 (0.430)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.495 (0.439)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.636 (0.231)</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.428 (0.496)</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.434 (0.445)</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.537 (0.136)</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.407 (0.492)</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0.373 (0.440)</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0.555 (0.215)</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>0.327 (0.469)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Run085</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.374 (0.440)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.592 (0.189)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0.320 (0.467)</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.293 (0.390)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.556 (0.202)</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.196 (0.398)</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.555 (0.440)</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.485 (0.156)</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.577 (0.495)</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>0.426 (0.443)</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>0.543 (0.186)</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>0.392 (0.488)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>Run086</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.488 (0.466)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0.641 (0.236)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0.452 (0.498)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0.504 (0.466)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0.784 (0.119)</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0.427 (0.496)</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0.684 (0.436)</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0.514 (0.178)</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>0.707 (0.455)</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>0.563 (0.464)</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0.640 (0.221)</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>0.547 (0.498)</t>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.592 (0.458)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.622 (0.242)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.585 (0.493)</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.482 (0.469)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.690 (0.197)</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.438 (0.498)</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.764 (0.387)</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.680 (0.178)</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.781 (0.414)</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0.652 (0.443)</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0.655 (0.213)</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0.651 (0.477)</t>
         </is>
       </c>
     </row>
@@ -714,7 +1274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -728,67 +1288,207 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Iteration22</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>0.59 (0.05)</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0.60 (0.06)</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>0.58 (0.08)</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>0.65 (0.07)</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>0.66 (0.03)</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>0.65 (0.12)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>0.58 (0.17)</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>0.59 (0.08)</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>0.58 (0.19)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>0.60 (0.06)</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>0.61 (0.04)</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>0.60 (0.06)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Iteration23</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.63 (0.12)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.66 (0.08)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.62 (0.14)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.79 (0.06)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.81 (0.03)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.78 (0.08)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.83 (0.06)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.66 (0.06)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.85 (0.07)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.73 (0.05)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0.70 (0.04)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.74 (0.07)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Iteration24</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.41 (0.11)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.55 (0.06)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.38 (0.13)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.49 (0.14)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.63 (0.05)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.44 (0.18)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.59 (0.12)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.57 (0.07)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.60 (0.13)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.49 (0.11)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.57 (0.05)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>0.47 (0.12)</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>0.60 (0.06)</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>0.43 (0.14)</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>0.55 (0.04)</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>0.77 (0.02)</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>0.47 (0.05)</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>0.69 (0.05)</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>0.67 (0.09)</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>0.68 (0.07)</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>0.56 (0.07)</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>0.66 (0.05)</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>0.53 (0.09)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changes in results display
</commit_message>
<xml_diff>
--- a/results/combined_output.xlsx
+++ b/results/combined_output.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,62 +434,62 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0.088 (0.172)</t>
+          <t>0.560 (0.449)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>0.320 (0.173)</t>
+          <t>0.455 (0.287)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0.002 (0.046)</t>
+          <t>0.600 (0.491)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>0.164 (0.264)</t>
+          <t>0.560 (0.428)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>0.390 (0.211)</t>
+          <t>0.580 (0.244)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>0.044 (0.205)</t>
+          <t>0.550 (0.499)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>0.121 (0.256)</t>
+          <t>0.768 (0.386)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>0.472 (0.171)</t>
+          <t>0.716 (0.210)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>0.041 (0.198)</t>
+          <t>0.779 (0.415)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>0.113 (0.225)</t>
+          <t>0.636 (0.435)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>0.378 (0.193)</t>
+          <t>0.555 (0.280)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>0.024 (0.153)</t>
+          <t>0.664 (0.473)</t>
         </is>
       </c>
     </row>
@@ -499,65 +499,345 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Run108</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.509 (0.444)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.758 (0.160)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.382 (0.486)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.617 (0.456)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.793 (0.197)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.564 (0.497)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.759 (0.414)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.607 (0.324)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.774 (0.419)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.613 (0.450)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0.745 (0.202)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.572 (0.495)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Run109</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.743 (0.383)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.733 (0.173)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.746 (0.436)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.776 (0.390)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.885 (0.100)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.741 (0.440)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.901 (0.260)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.801 (0.087)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.918 (0.275)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.807 (0.352)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.779 (0.156)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.814 (0.389)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Run110</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.720 (0.439)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.722 (0.169)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.719 (0.450)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.864 (0.299)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.875 (0.132)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.859 (0.349)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.816 (0.341)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.803 (0.141)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.820 (0.384)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0.781 (0.386)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0.809 (0.150)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.775 (0.418)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Run111</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.775 (0.394)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.872 (0.074)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.752 (0.432)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.810 (0.341)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.826 (0.159)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.802 (0.399)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.879 (0.307)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.676 (0.220)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.895 (0.307)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.819 (0.358)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0.826 (0.152)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.818 (0.386)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Run116</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>0.130 (0.214)</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>0.399 (0.183)</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>0.000 (0.000)</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>0.250 (0.323)</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>0.531 (0.216)</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>0.052 (0.223)</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>0.142 (0.288)</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>0.549 (0.176)</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>0.053 (0.224)</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>0.151 (0.266)</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>0.466 (0.201)</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>0.030 (0.172)</t>
         </is>
@@ -574,14 +854,85 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Iteration30</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>0.69 (0.10)</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0.77 (0.06)</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>0.65 (0.16)</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>0.77 (0.09)</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>0.84 (0.04)</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>0.74 (0.11)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>0.84 (0.06)</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>0.72 (0.08)</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>0.85 (0.06)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>0.75 (0.08)</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>0.79 (0.03)</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>0.74 (0.10)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
results from merging the networks
</commit_message>
<xml_diff>
--- a/results/combined_output.xlsx
+++ b/results/combined_output.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,67 +429,202 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Run105</t>
+          <t>Run076111114_final</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0.560 (0.449)</t>
+          <t>0.697 (0.394)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>0.455 (0.287)</t>
+          <t>0.688 (0.182)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>0.600 (0.491)</t>
+          <t>0.701 (0.459)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>0.560 (0.428)</t>
+          <t>0.787 (0.332)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>0.580 (0.244)</t>
+          <t>0.663 (0.197)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>0.550 (0.499)</t>
+          <t>0.844 (0.364)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>0.768 (0.386)</t>
+          <t>0.428 (0.455)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>0.716 (0.210)</t>
+          <t>0.586 (0.239)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>0.779 (0.415)</t>
+          <t>0.387 (0.488)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>0.636 (0.435)</t>
+          <t>0.628 (0.384)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>0.555 (0.280)</t>
+          <t>0.660 (0.212)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>0.664 (0.473)</t>
+          <t>0.598 (0.492)</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>0.631 (0.427)</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>0.646 (0.280)</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>0.623 (0.486)</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>0.178 (0.332)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>0.636 (0.185)</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>0.075 (0.264)</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>0.810 (0.335)</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>0.632 (0.261)</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>0.870 (0.337)</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>0.864 (0.306)</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>0.537 (0.277)</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>0.917 (0.276)</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>0.531 (0.486)</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>0.484 (0.228)</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>0.534 (0.499)</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>0.733 (0.375)</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>0.661 (0.221)</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>0.766 (0.423)</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>0.792 (0.351)</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>0.627 (0.247)</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>0.844 (0.363)</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>0.427 (0.467)</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>0.578 (0.230)</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>0.402 (0.490)</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>0.544 (0.388)</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>0.639 (0.211)</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>0.440 (0.497)</t>
         </is>
       </c>
     </row>
@@ -499,69 +634,96 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Run108</t>
+          <t>Run105</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.509 (0.444)</t>
+          <t>0.560 (0.449)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.758 (0.160)</t>
+          <t>0.455 (0.287)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.382 (0.486)</t>
+          <t>0.600 (0.491)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.617 (0.456)</t>
+          <t>0.560 (0.428)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.793 (0.197)</t>
+          <t>0.580 (0.244)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.564 (0.497)</t>
+          <t>0.550 (0.499)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.759 (0.414)</t>
+          <t>0.768 (0.386)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.607 (0.324)</t>
+          <t>0.716 (0.210)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.774 (0.419)</t>
+          <t>0.779 (0.415)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0.613 (0.450)</t>
+          <t>0.636 (0.435)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.745 (0.202)</t>
+          <t>0.555 (0.280)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.572 (0.495)</t>
-        </is>
-      </c>
+          <t>0.664 (0.473)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -569,69 +731,96 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Run109</t>
+          <t>Run108</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.743 (0.383)</t>
+          <t>0.509 (0.444)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.733 (0.173)</t>
+          <t>0.758 (0.160)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.746 (0.436)</t>
+          <t>0.382 (0.486)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.776 (0.390)</t>
+          <t>0.617 (0.456)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.885 (0.100)</t>
+          <t>0.793 (0.197)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.741 (0.440)</t>
+          <t>0.564 (0.497)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.901 (0.260)</t>
+          <t>0.759 (0.414)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.801 (0.087)</t>
+          <t>0.607 (0.324)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.918 (0.275)</t>
+          <t>0.774 (0.419)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.807 (0.352)</t>
+          <t>0.613 (0.450)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.779 (0.156)</t>
+          <t>0.745 (0.202)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.814 (0.389)</t>
-        </is>
-      </c>
+          <t>0.572 (0.495)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -639,69 +828,96 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Run110</t>
+          <t>Run109</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.720 (0.439)</t>
+          <t>0.743 (0.383)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.722 (0.169)</t>
+          <t>0.733 (0.173)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.719 (0.450)</t>
+          <t>0.746 (0.436)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.864 (0.299)</t>
+          <t>0.776 (0.390)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.875 (0.132)</t>
+          <t>0.885 (0.100)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.859 (0.349)</t>
+          <t>0.741 (0.440)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.816 (0.341)</t>
+          <t>0.901 (0.260)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.803 (0.141)</t>
+          <t>0.801 (0.087)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.820 (0.384)</t>
+          <t>0.918 (0.275)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0.781 (0.386)</t>
+          <t>0.807 (0.352)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.809 (0.150)</t>
+          <t>0.779 (0.156)</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.775 (0.418)</t>
-        </is>
-      </c>
+          <t>0.814 (0.389)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -709,69 +925,96 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Run111</t>
+          <t>Run110</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.775 (0.394)</t>
+          <t>0.720 (0.439)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.872 (0.074)</t>
+          <t>0.722 (0.169)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.752 (0.432)</t>
+          <t>0.719 (0.450)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.810 (0.341)</t>
+          <t>0.864 (0.299)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.826 (0.159)</t>
+          <t>0.875 (0.132)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.802 (0.399)</t>
+          <t>0.859 (0.349)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.879 (0.307)</t>
+          <t>0.816 (0.341)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.676 (0.220)</t>
+          <t>0.803 (0.141)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.895 (0.307)</t>
+          <t>0.820 (0.384)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.819 (0.358)</t>
+          <t>0.781 (0.386)</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.826 (0.152)</t>
+          <t>0.809 (0.150)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.818 (0.386)</t>
-        </is>
-      </c>
+          <t>0.775 (0.418)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -779,69 +1022,96 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Run112</t>
+          <t>Run111</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.357 (0.417)</t>
+          <t>0.775 (0.394)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.561 (0.199)</t>
+          <t>0.872 (0.074)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.282 (0.450)</t>
+          <t>0.752 (0.432)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.304 (0.428)</t>
+          <t>0.810 (0.341)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.720 (0.213)</t>
+          <t>0.826 (0.159)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.210 (0.408)</t>
+          <t>0.802 (0.399)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.456 (0.462)</t>
+          <t>0.879 (0.307)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.593 (0.169)</t>
+          <t>0.676 (0.220)</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.429 (0.496)</t>
+          <t>0.895 (0.307)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0.381 (0.438)</t>
+          <t>0.819 (0.358)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.594 (0.201)</t>
+          <t>0.826 (0.152)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.321 (0.467)</t>
-        </is>
-      </c>
+          <t>0.818 (0.386)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -849,69 +1119,96 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Run113</t>
+          <t>Run112</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.232 (0.368)</t>
+          <t>0.357 (0.417)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.581 (0.181)</t>
+          <t>0.561 (0.199)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.143 (0.351)</t>
+          <t>0.282 (0.450)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.305 (0.390)</t>
+          <t>0.304 (0.428)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.574 (0.236)</t>
+          <t>0.720 (0.213)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.180 (0.385)</t>
+          <t>0.210 (0.408)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.361 (0.410)</t>
+          <t>0.456 (0.462)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.568 (0.195)</t>
+          <t>0.593 (0.169)</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.272 (0.445)</t>
+          <t>0.429 (0.496)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0.292 (0.392)</t>
+          <t>0.381 (0.438)</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.574 (0.199)</t>
+          <t>0.594 (0.201)</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.193 (0.395)</t>
-        </is>
-      </c>
+          <t>0.321 (0.467)</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -919,69 +1216,96 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Run114</t>
+          <t>Run113</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.456 (0.466)</t>
+          <t>0.232 (0.368)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.648 (0.117)</t>
+          <t>0.581 (0.181)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.423 (0.495)</t>
+          <t>0.143 (0.351)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.345 (0.388)</t>
+          <t>0.305 (0.390)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.601 (0.237)</t>
+          <t>0.574 (0.236)</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.165 (0.373)</t>
+          <t>0.180 (0.385)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.588 (0.443)</t>
+          <t>0.361 (0.410)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.775 (0.135)</t>
+          <t>0.568 (0.195)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.511 (0.500)</t>
+          <t>0.272 (0.445)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0.499 (0.455)</t>
+          <t>0.292 (0.392)</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.703 (0.177)</t>
+          <t>0.574 (0.199)</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.432 (0.496)</t>
-        </is>
-      </c>
+          <t>0.193 (0.395)</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -989,69 +1313,96 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Run115</t>
+          <t>Run114</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.515 (0.466)</t>
+          <t>0.456 (0.466)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.620 (0.249)</t>
+          <t>0.648 (0.117)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.490 (0.500)</t>
+          <t>0.423 (0.495)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.558 (0.460)</t>
+          <t>0.345 (0.388)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.769 (0.116)</t>
+          <t>0.601 (0.237)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.500 (0.501)</t>
+          <t>0.165 (0.373)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.672 (0.441)</t>
+          <t>0.588 (0.443)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.529 (0.171)</t>
+          <t>0.775 (0.135)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.692 (0.462)</t>
+          <t>0.511 (0.500)</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>0.580 (0.461)</t>
+          <t>0.499 (0.455)</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.630 (0.222)</t>
+          <t>0.703 (0.177)</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.570 (0.495)</t>
-        </is>
-      </c>
+          <t>0.432 (0.496)</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1059,69 +1410,193 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Run115</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.515 (0.466)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.620 (0.249)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.490 (0.500)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.558 (0.460)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.769 (0.116)</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.500 (0.501)</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.672 (0.441)</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.529 (0.171)</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.692 (0.462)</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0.580 (0.461)</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>0.630 (0.222)</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>0.570 (0.495)</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>Run116</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>0.130 (0.214)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>0.399 (0.183)</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>0.000 (0.000)</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>0.250 (0.323)</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>0.531 (0.216)</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>0.052 (0.223)</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>0.142 (0.288)</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>0.549 (0.176)</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>0.053 (0.224)</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>0.151 (0.266)</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>0.466 (0.201)</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>0.030 (0.172)</t>
         </is>
       </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1293,14 +1768,75 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Run006</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>19.345775132275133 (0.3463753781829967)</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>23.063606382978723 (1.3582629963740993)</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>20.60390476190476 (0.8939518105016319)</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>21.233763492063492 (0.5747396061533153)</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>0.12837566137566137 (0.017411381174361588)</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>0.40445478723404255 (0.05662784312527957)</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>0.15325396825396825 (0.018307221707849142)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>0.21366031746031744 (0.03836058746689444)</t>
+        </is>
+      </c>
+      <c r="J1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>20.55998327759197 (1.523727171523039)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>0.19685576923076925 (0.10171105620616296)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
results from processed masks
</commit_message>
<xml_diff>
--- a/results/combined_output.xlsx
+++ b/results/combined_output.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO17"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,107 +567,107 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.191 (0.378)</t>
+          <t>0.522 (0.490)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.475 (0.270)</t>
+          <t>0.694 (0.220)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.170 (0.377)</t>
+          <t>0.509 (0.502)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.455 (0.418)</t>
+          <t>0.676 (0.379)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.533 (0.230)</t>
+          <t>0.559 (0.209)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.408 (0.495)</t>
+          <t>0.746 (0.438)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.132 (0.339)</t>
+          <t>0.386 (0.489)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.023 (0.032)</t>
+          <t>0.011 (0.016)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.134 (0.342)</t>
+          <t>0.393 (0.491)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0.191 (0.378)</t>
+          <t>0.522 (0.490)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.475 (0.270)</t>
+          <t>0.694 (0.220)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.170 (0.377)</t>
+          <t>0.509 (0.502)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>0.455 (0.418)</t>
+          <t>0.676 (0.379)</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0.533 (0.230)</t>
+          <t>0.559 (0.209)</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>0.408 (0.495)</t>
+          <t>0.746 (0.438)</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>0.132 (0.339)</t>
+          <t>0.386 (0.489)</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>0.023 (0.032)</t>
+          <t>0.011 (0.016)</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>0.134 (0.342)</t>
+          <t>0.393 (0.491)</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>0.176 (0.261)</t>
+          <t>0.399 (0.395)</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>0.300 (0.187)</t>
+          <t>0.409 (0.219)</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>0.078 (0.270)</t>
+          <t>0.391 (0.492)</t>
         </is>
       </c>
       <c r="X2" t="inlineStr"/>
@@ -700,199 +700,127 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.740 (0.370)</t>
+          <t>0.191 (0.378)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.431 (0.256)</t>
+          <t>0.475 (0.270)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.879 (0.327)</t>
+          <t>0.170 (0.377)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.896 (0.214)</t>
+          <t>0.455 (0.418)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.762 (0.173)</t>
+          <t>0.533 (0.230)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.957 (0.202)</t>
+          <t>0.408 (0.495)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.903 (0.236)</t>
+          <t>0.132 (0.339)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.710 (0.225)</t>
+          <t>0.023 (0.032)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.953 (0.211)</t>
+          <t>0.134 (0.342)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.307 (0.358)</t>
+          <t>0.191 (0.378)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.315 (0.200)</t>
+          <t>0.475 (0.270)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.299 (0.460)</t>
+          <t>0.170 (0.377)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>0.707 (0.410)</t>
+          <t>0.455 (0.418)</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>0.580 (0.357)</t>
+          <t>0.533 (0.230)</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>0.772 (0.421)</t>
+          <t>0.408 (0.495)</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>0.850 (0.304)</t>
+          <t>0.132 (0.339)</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>0.627 (0.202)</t>
+          <t>0.023 (0.032)</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>0.900 (0.301)</t>
+          <t>0.134 (0.342)</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>0.763 (0.369)</t>
+          <t>0.176 (0.261)</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>0.457 (0.271)</t>
+          <t>0.300 (0.187)</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>0.867 (0.339)</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>0.870 (0.304)</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>0.670 (0.276)</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>0.903 (0.296)</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>0.726 (0.433)</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>0.538 (0.254)</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>0.738 (0.440)</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>0.671 (0.406)</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>0.407 (0.253)</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>0.793 (0.406)</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>0.850 (0.305)</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>0.692 (0.268)</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>0.901 (0.299)</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>0.816 (0.355)</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>0.656 (0.235)</t>
-        </is>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>0.843 (0.364)</t>
-        </is>
-      </c>
-      <c r="AM3" t="inlineStr">
-        <is>
-          <t>0.627 (0.380)</t>
-        </is>
-      </c>
-      <c r="AN3" t="inlineStr">
-        <is>
-          <t>0.542 (0.280)</t>
-        </is>
-      </c>
-      <c r="AO3" t="inlineStr">
-        <is>
-          <t>0.722 (0.449)</t>
-        </is>
-      </c>
+          <t>0.078 (0.270)</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -905,197 +833,197 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.852 (0.261)</t>
+          <t>0.740 (0.370)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.654 (0.195)</t>
+          <t>0.431 (0.256)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.941 (0.237)</t>
+          <t>0.879 (0.327)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.918 (0.182)</t>
+          <t>0.896 (0.214)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.799 (0.156)</t>
+          <t>0.762 (0.173)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.972 (0.166)</t>
+          <t>0.957 (0.202)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.934 (0.180)</t>
+          <t>0.903 (0.236)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.767 (0.197)</t>
+          <t>0.710 (0.225)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.978 (0.147)</t>
+          <t>0.953 (0.211)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0.645 (0.383)</t>
+          <t>0.307 (0.358)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.645 (0.238)</t>
+          <t>0.315 (0.200)</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.646 (0.480)</t>
+          <t>0.299 (0.460)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>0.821 (0.331)</t>
+          <t>0.707 (0.410)</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>0.687 (0.322)</t>
+          <t>0.580 (0.357)</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>0.889 (0.315)</t>
+          <t>0.772 (0.421)</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>0.852 (0.310)</t>
+          <t>0.850 (0.304)</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>0.703 (0.209)</t>
+          <t>0.627 (0.202)</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>0.885 (0.320)</t>
+          <t>0.900 (0.301)</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>0.818 (0.330)</t>
+          <t>0.763 (0.369)</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>0.624 (0.278)</t>
+          <t>0.457 (0.271)</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>0.884 (0.321)</t>
+          <t>0.867 (0.339)</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>0.929 (0.215)</t>
+          <t>0.870 (0.304)</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>0.744 (0.229)</t>
+          <t>0.670 (0.276)</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>0.960 (0.197)</t>
+          <t>0.903 (0.296)</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>0.755 (0.415)</t>
+          <t>0.726 (0.433)</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>0.588 (0.204)</t>
+          <t>0.538 (0.254)</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>0.766 (0.424)</t>
+          <t>0.738 (0.440)</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>0.799 (0.325)</t>
+          <t>0.671 (0.406)</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>0.641 (0.238)</t>
+          <t>0.407 (0.253)</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>0.873 (0.334)</t>
+          <t>0.793 (0.406)</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>0.905 (0.233)</t>
+          <t>0.850 (0.305)</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>0.756 (0.231)</t>
+          <t>0.692 (0.268)</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>0.952 (0.213)</t>
+          <t>0.901 (0.299)</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>0.841 (0.333)</t>
+          <t>0.816 (0.355)</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>0.716 (0.212)</t>
+          <t>0.656 (0.235)</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>0.862 (0.345)</t>
+          <t>0.843 (0.364)</t>
         </is>
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>0.742 (0.326)</t>
+          <t>0.627 (0.380)</t>
         </is>
       </c>
       <c r="AN4" t="inlineStr">
         <is>
-          <t>0.702 (0.218)</t>
+          <t>0.542 (0.280)</t>
         </is>
       </c>
       <c r="AO4" t="inlineStr">
         <is>
-          <t>0.786 (0.410)</t>
+          <t>0.722 (0.449)</t>
         </is>
       </c>
     </row>
@@ -1105,112 +1033,112 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Run076111114_final</t>
+          <t>Run058_final</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.046 (0.178)</t>
+          <t>0.530 (0.489)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.403 (0.274)</t>
+          <t>0.681 (0.218)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.019 (0.137)</t>
+          <t>0.519 (0.502)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.498 (0.412)</t>
+          <t>0.681 (0.377)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.460 (0.178)</t>
+          <t>0.551 (0.213)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.521 (0.503)</t>
+          <t>0.761 (0.430)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.001 (0.008)</t>
+          <t>0.404 (0.492)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.054 (0.037)</t>
+          <t>0.023 (0.032)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.000 (0.000)</t>
+          <t>0.411 (0.494)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.046 (0.178)</t>
+          <t>0.530 (0.489)</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.403 (0.274)</t>
+          <t>0.681 (0.218)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>0.019 (0.137)</t>
+          <t>0.519 (0.502)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.498 (0.412)</t>
+          <t>0.681 (0.377)</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.460 (0.178)</t>
+          <t>0.551 (0.213)</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>0.521 (0.503)</t>
+          <t>0.761 (0.430)</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>0.001 (0.008)</t>
+          <t>0.404 (0.492)</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>0.054 (0.037)</t>
+          <t>0.023 (0.032)</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>0.000 (0.000)</t>
+          <t>0.411 (0.494)</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>0.079 (0.123)</t>
+          <t>0.358 (0.385)</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>0.180 (0.128)</t>
+          <t>0.397 (0.225)</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>0.000 (0.000)</t>
+          <t>0.328 (0.473)</t>
         </is>
       </c>
       <c r="X5" t="inlineStr"/>
@@ -1238,202 +1166,202 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Run076111114_final</t>
+          <t>Run058_final</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.697 (0.394)</t>
+          <t>0.852 (0.261)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.688 (0.182)</t>
+          <t>0.654 (0.195)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.701 (0.459)</t>
+          <t>0.941 (0.237)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.787 (0.332)</t>
+          <t>0.918 (0.182)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.663 (0.197)</t>
+          <t>0.799 (0.156)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.844 (0.364)</t>
+          <t>0.972 (0.166)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.428 (0.455)</t>
+          <t>0.934 (0.180)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.586 (0.239)</t>
+          <t>0.767 (0.197)</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.387 (0.488)</t>
+          <t>0.978 (0.147)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0.628 (0.384)</t>
+          <t>0.645 (0.383)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.660 (0.212)</t>
+          <t>0.645 (0.238)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.598 (0.492)</t>
+          <t>0.646 (0.480)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>0.631 (0.427)</t>
+          <t>0.821 (0.331)</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>0.646 (0.280)</t>
+          <t>0.687 (0.322)</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>0.623 (0.486)</t>
+          <t>0.889 (0.315)</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>0.178 (0.332)</t>
+          <t>0.852 (0.310)</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>0.636 (0.185)</t>
+          <t>0.703 (0.209)</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>0.075 (0.264)</t>
+          <t>0.885 (0.320)</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>0.810 (0.335)</t>
+          <t>0.818 (0.330)</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>0.632 (0.261)</t>
+          <t>0.624 (0.278)</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>0.870 (0.337)</t>
+          <t>0.884 (0.321)</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>0.864 (0.306)</t>
+          <t>0.929 (0.215)</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>0.537 (0.277)</t>
+          <t>0.744 (0.229)</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>0.917 (0.276)</t>
+          <t>0.960 (0.197)</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>0.531 (0.486)</t>
+          <t>0.755 (0.415)</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>0.484 (0.228)</t>
+          <t>0.588 (0.204)</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>0.534 (0.499)</t>
+          <t>0.766 (0.424)</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>0.733 (0.375)</t>
+          <t>0.799 (0.325)</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>0.661 (0.221)</t>
+          <t>0.641 (0.238)</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>0.766 (0.423)</t>
+          <t>0.873 (0.334)</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>0.792 (0.351)</t>
+          <t>0.905 (0.233)</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>0.627 (0.247)</t>
+          <t>0.756 (0.231)</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>0.844 (0.363)</t>
+          <t>0.952 (0.213)</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>0.427 (0.467)</t>
+          <t>0.841 (0.333)</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>0.578 (0.230)</t>
+          <t>0.716 (0.212)</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>0.402 (0.490)</t>
+          <t>0.862 (0.345)</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>0.544 (0.388)</t>
+          <t>0.742 (0.326)</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>0.639 (0.211)</t>
+          <t>0.702 (0.218)</t>
         </is>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>0.440 (0.497)</t>
+          <t>0.786 (0.410)</t>
         </is>
       </c>
     </row>
@@ -1448,42 +1376,42 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.038 (0.155)</t>
+          <t>0.046 (0.178)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.412 (0.274)</t>
+          <t>0.403 (0.274)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.009 (0.097)</t>
+          <t>0.019 (0.137)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.563 (0.407)</t>
+          <t>0.498 (0.412)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.468 (0.183)</t>
+          <t>0.460 (0.178)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.620 (0.489)</t>
+          <t>0.521 (0.503)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.001 (0.007)</t>
+          <t>0.001 (0.008)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.040 (0.041)</t>
+          <t>0.054 (0.037)</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1493,42 +1421,42 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0.038 (0.155)</t>
+          <t>0.046 (0.178)</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.412 (0.274)</t>
+          <t>0.403 (0.274)</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>0.009 (0.097)</t>
+          <t>0.019 (0.137)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.563 (0.407)</t>
+          <t>0.498 (0.412)</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.468 (0.183)</t>
+          <t>0.460 (0.178)</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>0.620 (0.489)</t>
+          <t>0.521 (0.503)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>0.001 (0.007)</t>
+          <t>0.001 (0.008)</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>0.040 (0.041)</t>
+          <t>0.054 (0.037)</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1538,12 +1466,12 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>0.078 (0.122)</t>
+          <t>0.079 (0.123)</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>0.178 (0.127)</t>
+          <t>0.180 (0.128)</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1576,78 +1504,114 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Run105</t>
+          <t>Run076111114_final</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.560 (0.449)</t>
+          <t>0.455 (0.487)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.455 (0.287)</t>
+          <t>0.605 (0.253)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.600 (0.491)</t>
+          <t>0.443 (0.499)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.560 (0.428)</t>
+          <t>0.579 (0.402)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.580 (0.244)</t>
+          <t>0.466 (0.171)</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.550 (0.499)</t>
+          <t>0.648 (0.481)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.768 (0.386)</t>
+          <t>0.230 (0.421)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.716 (0.210)</t>
+          <t>0.096 (0.015)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.779 (0.415)</t>
+          <t>0.232 (0.424)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0.636 (0.435)</t>
+          <t>0.455 (0.487)</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.555 (0.280)</t>
+          <t>0.605 (0.253)</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>0.664 (0.473)</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
+          <t>0.443 (0.499)</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.579 (0.402)</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0.466 (0.171)</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>0.648 (0.481)</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>0.230 (0.421)</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>0.096 (0.015)</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>0.232 (0.424)</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0.222 (0.307)</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>0.287 (0.153)</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>0.172 (0.380)</t>
+        </is>
+      </c>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr"/>
@@ -1673,96 +1637,204 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Run108</t>
+          <t>Run076111114_final</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.509 (0.444)</t>
+          <t>0.697 (0.394)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.758 (0.160)</t>
+          <t>0.688 (0.182)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.382 (0.486)</t>
+          <t>0.701 (0.459)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.617 (0.456)</t>
+          <t>0.787 (0.332)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.793 (0.197)</t>
+          <t>0.663 (0.197)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.564 (0.497)</t>
+          <t>0.844 (0.364)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.759 (0.414)</t>
+          <t>0.428 (0.455)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.607 (0.324)</t>
+          <t>0.586 (0.239)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.774 (0.419)</t>
+          <t>0.387 (0.488)</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>0.613 (0.450)</t>
+          <t>0.628 (0.384)</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.745 (0.202)</t>
+          <t>0.660 (0.212)</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>0.572 (0.495)</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="inlineStr"/>
-      <c r="AL9" t="inlineStr"/>
-      <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr"/>
-      <c r="AO9" t="inlineStr"/>
+          <t>0.598 (0.492)</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0.631 (0.427)</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0.646 (0.280)</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>0.623 (0.486)</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>0.178 (0.332)</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0.636 (0.185)</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>0.075 (0.264)</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0.810 (0.335)</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>0.632 (0.261)</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>0.870 (0.337)</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>0.864 (0.306)</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>0.537 (0.277)</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>0.917 (0.276)</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>0.531 (0.486)</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>0.484 (0.228)</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>0.534 (0.499)</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>0.733 (0.375)</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>0.661 (0.221)</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>0.766 (0.423)</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>0.792 (0.351)</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>0.627 (0.247)</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>0.844 (0.363)</t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>0.427 (0.467)</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>0.578 (0.230)</t>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>0.402 (0.490)</t>
+        </is>
+      </c>
+      <c r="AM9" t="inlineStr">
+        <is>
+          <t>0.544 (0.388)</t>
+        </is>
+      </c>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>0.639 (0.211)</t>
+        </is>
+      </c>
+      <c r="AO9" t="inlineStr">
+        <is>
+          <t>0.440 (0.497)</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1770,78 +1842,114 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Run109</t>
+          <t>Run076111114_final</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.743 (0.383)</t>
+          <t>0.038 (0.155)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.733 (0.173)</t>
+          <t>0.412 (0.274)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.746 (0.436)</t>
+          <t>0.009 (0.097)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.776 (0.390)</t>
+          <t>0.563 (0.407)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.885 (0.100)</t>
+          <t>0.468 (0.183)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.741 (0.440)</t>
+          <t>0.620 (0.489)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.901 (0.260)</t>
+          <t>0.001 (0.007)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.801 (0.087)</t>
+          <t>0.040 (0.041)</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.918 (0.275)</t>
+          <t>0.000 (0.000)</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>0.807 (0.352)</t>
+          <t>0.038 (0.155)</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.779 (0.156)</t>
+          <t>0.412 (0.274)</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.814 (0.389)</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
+          <t>0.009 (0.097)</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.563 (0.407)</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0.468 (0.183)</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>0.620 (0.489)</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>0.001 (0.007)</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0.040 (0.041)</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>0.000 (0.000)</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>0.078 (0.122)</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>0.178 (0.127)</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>0.000 (0.000)</t>
+        </is>
+      </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr"/>
@@ -1867,78 +1975,114 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Run110</t>
+          <t>Run076111114_final</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.720 (0.439)</t>
+          <t>0.487 (0.489)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.722 (0.169)</t>
+          <t>0.683 (0.208)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.719 (0.450)</t>
+          <t>0.472 (0.502)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.864 (0.299)</t>
+          <t>0.593 (0.399)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.875 (0.132)</t>
+          <t>0.479 (0.172)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.859 (0.349)</t>
+          <t>0.662 (0.476)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.816 (0.341)</t>
+          <t>0.273 (0.447)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.803 (0.141)</t>
+          <t>0.041 (0.043)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.820 (0.384)</t>
+          <t>0.277 (0.449)</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0.781 (0.386)</t>
+          <t>0.487 (0.489)</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.809 (0.150)</t>
+          <t>0.683 (0.208)</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>0.775 (0.418)</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
+          <t>0.472 (0.502)</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>0.593 (0.399)</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0.479 (0.172)</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0.662 (0.476)</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>0.273 (0.447)</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0.041 (0.043)</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>0.277 (0.449)</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0.248 (0.328)</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>0.285 (0.151)</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>0.219 (0.417)</t>
+        </is>
+      </c>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
@@ -1964,67 +2108,67 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Run111</t>
+          <t>Run105</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.775 (0.394)</t>
+          <t>0.560 (0.449)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.872 (0.074)</t>
+          <t>0.455 (0.287)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.752 (0.432)</t>
+          <t>0.600 (0.491)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.810 (0.341)</t>
+          <t>0.560 (0.428)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.826 (0.159)</t>
+          <t>0.580 (0.244)</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.802 (0.399)</t>
+          <t>0.550 (0.499)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.879 (0.307)</t>
+          <t>0.768 (0.386)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0.676 (0.220)</t>
+          <t>0.716 (0.210)</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0.895 (0.307)</t>
+          <t>0.779 (0.415)</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>0.819 (0.358)</t>
+          <t>0.636 (0.435)</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.826 (0.152)</t>
+          <t>0.555 (0.280)</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0.818 (0.386)</t>
+          <t>0.664 (0.473)</t>
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
@@ -2061,67 +2205,67 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Run112</t>
+          <t>Run108</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.357 (0.417)</t>
+          <t>0.509 (0.444)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.561 (0.199)</t>
+          <t>0.758 (0.160)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.282 (0.450)</t>
+          <t>0.382 (0.486)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.304 (0.428)</t>
+          <t>0.617 (0.456)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0.720 (0.213)</t>
+          <t>0.793 (0.197)</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.210 (0.408)</t>
+          <t>0.564 (0.497)</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.456 (0.462)</t>
+          <t>0.759 (0.414)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0.593 (0.169)</t>
+          <t>0.607 (0.324)</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0.429 (0.496)</t>
+          <t>0.774 (0.419)</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>0.381 (0.438)</t>
+          <t>0.613 (0.450)</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0.594 (0.201)</t>
+          <t>0.745 (0.202)</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>0.321 (0.467)</t>
+          <t>0.572 (0.495)</t>
         </is>
       </c>
       <c r="O13" t="inlineStr"/>
@@ -2158,67 +2302,67 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Run113</t>
+          <t>Run109</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.232 (0.368)</t>
+          <t>0.743 (0.383)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.581 (0.181)</t>
+          <t>0.733 (0.173)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.143 (0.351)</t>
+          <t>0.746 (0.436)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.305 (0.390)</t>
+          <t>0.776 (0.390)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.574 (0.236)</t>
+          <t>0.885 (0.100)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.180 (0.385)</t>
+          <t>0.741 (0.440)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.361 (0.410)</t>
+          <t>0.901 (0.260)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.568 (0.195)</t>
+          <t>0.801 (0.087)</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0.272 (0.445)</t>
+          <t>0.918 (0.275)</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>0.292 (0.392)</t>
+          <t>0.807 (0.352)</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0.574 (0.199)</t>
+          <t>0.779 (0.156)</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>0.193 (0.395)</t>
+          <t>0.814 (0.389)</t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
@@ -2255,67 +2399,67 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Run114</t>
+          <t>Run110</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.456 (0.466)</t>
+          <t>0.720 (0.439)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.648 (0.117)</t>
+          <t>0.722 (0.169)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.423 (0.495)</t>
+          <t>0.719 (0.450)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.345 (0.388)</t>
+          <t>0.864 (0.299)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.601 (0.237)</t>
+          <t>0.875 (0.132)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.165 (0.373)</t>
+          <t>0.859 (0.349)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.588 (0.443)</t>
+          <t>0.816 (0.341)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.775 (0.135)</t>
+          <t>0.803 (0.141)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>0.511 (0.500)</t>
+          <t>0.820 (0.384)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0.499 (0.455)</t>
+          <t>0.781 (0.386)</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>0.703 (0.177)</t>
+          <t>0.809 (0.150)</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>0.432 (0.496)</t>
+          <t>0.775 (0.418)</t>
         </is>
       </c>
       <c r="O15" t="inlineStr"/>
@@ -2352,67 +2496,67 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Run115</t>
+          <t>Run111</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.515 (0.466)</t>
+          <t>0.775 (0.394)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.620 (0.249)</t>
+          <t>0.872 (0.074)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.490 (0.500)</t>
+          <t>0.752 (0.432)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0.558 (0.460)</t>
+          <t>0.810 (0.341)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.769 (0.116)</t>
+          <t>0.826 (0.159)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.500 (0.501)</t>
+          <t>0.802 (0.399)</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.672 (0.441)</t>
+          <t>0.879 (0.307)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.529 (0.171)</t>
+          <t>0.676 (0.220)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0.692 (0.462)</t>
+          <t>0.895 (0.307)</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>0.580 (0.461)</t>
+          <t>0.819 (0.358)</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>0.630 (0.222)</t>
+          <t>0.826 (0.152)</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>0.570 (0.495)</t>
+          <t>0.818 (0.386)</t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>
@@ -2449,67 +2593,67 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Run116</t>
+          <t>Run112</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.130 (0.214)</t>
+          <t>0.357 (0.417)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.399 (0.183)</t>
+          <t>0.561 (0.199)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.000 (0.000)</t>
+          <t>0.282 (0.450)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0.250 (0.323)</t>
+          <t>0.304 (0.428)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.531 (0.216)</t>
+          <t>0.720 (0.213)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0.052 (0.223)</t>
+          <t>0.210 (0.408)</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.142 (0.288)</t>
+          <t>0.456 (0.462)</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.549 (0.176)</t>
+          <t>0.593 (0.169)</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>0.053 (0.224)</t>
+          <t>0.429 (0.496)</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>0.151 (0.266)</t>
+          <t>0.381 (0.438)</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.466 (0.201)</t>
+          <t>0.594 (0.201)</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>0.030 (0.172)</t>
+          <t>0.321 (0.467)</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
@@ -2540,6 +2684,394 @@
       <c r="AN17" t="inlineStr"/>
       <c r="AO17" t="inlineStr"/>
     </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Run113</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0.232 (0.368)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.581 (0.181)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0.143 (0.351)</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0.305 (0.390)</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0.574 (0.236)</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.180 (0.385)</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.361 (0.410)</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.568 (0.195)</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.272 (0.445)</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>0.292 (0.392)</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>0.574 (0.199)</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>0.193 (0.395)</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr"/>
+      <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Run114</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.456 (0.466)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.648 (0.117)</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0.423 (0.495)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0.345 (0.388)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0.601 (0.237)</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0.165 (0.373)</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.588 (0.443)</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0.775 (0.135)</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0.511 (0.500)</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>0.499 (0.455)</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>0.703 (0.177)</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>0.432 (0.496)</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr"/>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Run115</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.515 (0.466)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.620 (0.249)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0.490 (0.500)</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0.558 (0.460)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0.769 (0.116)</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0.500 (0.501)</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.672 (0.441)</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.529 (0.171)</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0.692 (0.462)</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>0.580 (0.461)</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>0.630 (0.222)</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>0.570 (0.495)</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+      <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="inlineStr"/>
+      <c r="AJ20" t="inlineStr"/>
+      <c r="AK20" t="inlineStr"/>
+      <c r="AL20" t="inlineStr"/>
+      <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
+      <c r="AO20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Run116</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.130 (0.214)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.399 (0.183)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.000 (0.000)</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0.250 (0.323)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0.531 (0.216)</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0.052 (0.223)</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0.142 (0.288)</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.549 (0.176)</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0.053 (0.224)</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>0.151 (0.266)</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>0.466 (0.201)</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>0.030 (0.172)</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="inlineStr"/>
+      <c r="AK21" t="inlineStr"/>
+      <c r="AL21" t="inlineStr"/>
+      <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr"/>
+      <c r="AO21" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>